<commit_message>
added ATF fsh CV
</commit_message>
<xml_diff>
--- a/GOA/GOA_2018_SS.xlsx
+++ b/GOA/GOA_2018_SS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantadams/Documents/GitHub/RceattleRuns/GOA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE478335-2113-0844-8B7F-43A78417F686}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0893009A-C687-474A-9DE0-D34B26CE2352}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13920" activeTab="10" xr2:uid="{075EC1A9-A118-934F-9672-DCD5B7DE9E6F}"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13920" activeTab="2" xr2:uid="{075EC1A9-A118-934F-9672-DCD5B7DE9E6F}"/>
   </bookViews>
   <sheets>
     <sheet name="control" sheetId="8" r:id="rId1"/>
@@ -1132,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7F6EB4-5D4F-BC45-969E-AE3CAB6A8489}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
@@ -1494,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D070E12-05E4-2C43-8D2E-82B50EB451CB}">
   <dimension ref="A1:BE107"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="P111" sqref="P111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2767,6 +2767,9 @@
       <c r="F51">
         <v>514</v>
       </c>
+      <c r="G51">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
@@ -2787,6 +2790,9 @@
       <c r="F52">
         <v>514</v>
       </c>
+      <c r="G52">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="4" t="s">
@@ -2807,6 +2813,9 @@
       <c r="F53">
         <v>514</v>
       </c>
+      <c r="G53">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="4" t="s">
@@ -2827,6 +2836,9 @@
       <c r="F54">
         <v>514</v>
       </c>
+      <c r="G54">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="4" t="s">
@@ -2847,6 +2859,9 @@
       <c r="F55">
         <v>514</v>
       </c>
+      <c r="G55">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="4" t="s">
@@ -2867,6 +2882,9 @@
       <c r="F56">
         <v>2469</v>
       </c>
+      <c r="G56">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="4" t="s">
@@ -2887,6 +2905,9 @@
       <c r="F57">
         <v>2276</v>
       </c>
+      <c r="G57">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="4" t="s">
@@ -2907,6 +2928,9 @@
       <c r="F58">
         <v>1697</v>
       </c>
+      <c r="G58">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="4" t="s">
@@ -2927,6 +2951,9 @@
       <c r="F59">
         <v>1315</v>
       </c>
+      <c r="G59">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="4" t="s">
@@ -2947,6 +2974,9 @@
       <c r="F60">
         <v>1886</v>
       </c>
+      <c r="G60">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="4" t="s">
@@ -2967,6 +2997,9 @@
       <c r="F61">
         <v>1185</v>
       </c>
+      <c r="G61">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="4" t="s">
@@ -2987,6 +3020,9 @@
       <c r="F62">
         <v>4477</v>
       </c>
+      <c r="G62">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="4" t="s">
@@ -3007,6 +3043,9 @@
       <c r="F63">
         <v>10007</v>
       </c>
+      <c r="G63">
+        <v>0.70710680000000004</v>
+      </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="4" t="s">
@@ -3027,8 +3066,11 @@
       <c r="F64">
         <v>4883</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="4" t="s">
         <v>75</v>
       </c>
@@ -3047,8 +3089,11 @@
       <c r="F65">
         <v>2776</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="4" t="s">
         <v>75</v>
       </c>
@@ -3067,8 +3112,11 @@
       <c r="F66">
         <v>3045</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="4" t="s">
         <v>75</v>
       </c>
@@ -3087,8 +3135,11 @@
       <c r="F67">
         <v>9449</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="4" t="s">
         <v>75</v>
       </c>
@@ -3107,8 +3158,11 @@
       <c r="F68">
         <v>8409</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="4" t="s">
         <v>75</v>
       </c>
@@ -3127,8 +3181,11 @@
       <c r="F69">
         <v>7579</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="4" t="s">
         <v>75</v>
       </c>
@@ -3147,8 +3204,11 @@
       <c r="F70">
         <v>7848</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="4" t="s">
         <v>75</v>
       </c>
@@ -3167,8 +3227,11 @@
       <c r="F71">
         <v>7433</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="4" t="s">
         <v>75</v>
       </c>
@@ -3187,8 +3250,11 @@
       <c r="F72">
         <v>4639</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="4" t="s">
         <v>75</v>
       </c>
@@ -3207,8 +3273,11 @@
       <c r="F73">
         <v>6331</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="4" t="s">
         <v>75</v>
       </c>
@@ -3227,8 +3296,11 @@
       <c r="F74">
         <v>3457</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="4" t="s">
         <v>75</v>
       </c>
@@ -3247,8 +3319,11 @@
       <c r="F75">
         <v>1539</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="4" t="s">
         <v>75</v>
       </c>
@@ -3267,8 +3342,11 @@
       <c r="F76">
         <v>1221</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="4" t="s">
         <v>75</v>
       </c>
@@ -3287,8 +3365,11 @@
       <c r="F77">
         <v>4963</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" s="4" t="s">
         <v>75</v>
       </c>
@@ -3307,8 +3388,11 @@
       <c r="F78">
         <v>5138</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="4" t="s">
         <v>75</v>
       </c>
@@ -3327,8 +3411,11 @@
       <c r="F79">
         <v>2584</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="4" t="s">
         <v>75</v>
       </c>
@@ -3347,8 +3434,11 @@
       <c r="F80">
         <v>7706</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="4" t="s">
         <v>75</v>
       </c>
@@ -3367,8 +3457,11 @@
       <c r="F81">
         <v>10034</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="4" t="s">
         <v>75</v>
       </c>
@@ -3387,8 +3480,11 @@
       <c r="F82">
         <v>15970</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="G82">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="4" t="s">
         <v>75</v>
       </c>
@@ -3407,8 +3503,11 @@
       <c r="F83">
         <v>15559</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="G83">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="4" t="s">
         <v>75</v>
       </c>
@@ -3427,8 +3526,11 @@
       <c r="F84">
         <v>23560</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="G84">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="4" t="s">
         <v>75</v>
       </c>
@@ -3447,8 +3549,11 @@
       <c r="F85">
         <v>18428</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="G85">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="4" t="s">
         <v>75</v>
       </c>
@@ -3467,8 +3572,11 @@
       <c r="F86">
         <v>22583</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="G86">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" s="4" t="s">
         <v>75</v>
       </c>
@@ -3487,8 +3595,11 @@
       <c r="F87">
         <v>16319</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="G87">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" s="4" t="s">
         <v>75</v>
       </c>
@@ -3507,8 +3618,11 @@
       <c r="F88">
         <v>12975</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="G88">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="4" t="s">
         <v>75</v>
       </c>
@@ -3527,8 +3641,11 @@
       <c r="F89">
         <v>16207</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="G89">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" s="4" t="s">
         <v>75</v>
       </c>
@@ -3547,8 +3664,11 @@
       <c r="F90">
         <v>24252</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="G90">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="4" t="s">
         <v>75</v>
       </c>
@@ -3567,8 +3687,11 @@
       <c r="F91">
         <v>19964</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="G91">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="4" t="s">
         <v>75</v>
       </c>
@@ -3587,8 +3710,11 @@
       <c r="F92">
         <v>21231</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="G92">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" s="4" t="s">
         <v>75</v>
       </c>
@@ -3607,8 +3733,11 @@
       <c r="F93">
         <v>29994</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="G93">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="4" t="s">
         <v>75</v>
       </c>
@@ -3627,8 +3756,11 @@
       <c r="F94">
         <v>15304</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="G94">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" s="4" t="s">
         <v>75</v>
       </c>
@@ -3647,8 +3779,11 @@
       <c r="F95">
         <v>19770</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="G95">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="4" t="s">
         <v>75</v>
       </c>
@@ -3667,8 +3802,11 @@
       <c r="F96">
         <v>27653</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="G96">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" s="4" t="s">
         <v>75</v>
       </c>
@@ -3687,8 +3825,11 @@
       <c r="F97">
         <v>25494</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="G97">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" s="4" t="s">
         <v>75</v>
       </c>
@@ -3707,8 +3848,11 @@
       <c r="F98">
         <v>29293</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="G98">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" s="4" t="s">
         <v>75</v>
       </c>
@@ -3727,8 +3871,11 @@
       <c r="F99">
         <v>24937</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="G99">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" s="4" t="s">
         <v>75</v>
       </c>
@@ -3747,8 +3894,11 @@
       <c r="F100">
         <v>24094</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="G100">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" s="4" t="s">
         <v>75</v>
       </c>
@@ -3767,8 +3917,11 @@
       <c r="F101">
         <v>31009</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="G101">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" s="4" t="s">
         <v>75</v>
       </c>
@@ -3787,8 +3940,11 @@
       <c r="F102">
         <v>20566</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="G102">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103" s="4" t="s">
         <v>75</v>
       </c>
@@ -3807,8 +3963,11 @@
       <c r="F103">
         <v>21608</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="G103">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" s="4" t="s">
         <v>75</v>
       </c>
@@ -3827,8 +3986,11 @@
       <c r="F104">
         <v>36294</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="G104">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105" s="4" t="s">
         <v>75</v>
       </c>
@@ -3847,8 +4009,11 @@
       <c r="F105">
         <v>19055</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="G105">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106" s="4" t="s">
         <v>75</v>
       </c>
@@ -3867,8 +4032,11 @@
       <c r="F106">
         <v>19830</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
+      <c r="G106">
+        <v>0.70710680000000004</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107" s="4" t="s">
         <v>75</v>
       </c>
@@ -3886,6 +4054,9 @@
       </c>
       <c r="F107">
         <v>20283</v>
+      </c>
+      <c r="G107">
+        <v>0.70710680000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>